<commit_message>
Main estimation done but to be tested
</commit_message>
<xml_diff>
--- a/src/preprocessing/term-document matrix/FOMC1_dictionary_meeting_onlyTF.xlsx
+++ b/src/preprocessing/term-document matrix/FOMC1_dictionary_meeting_onlyTF.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202">
   <si>
     <t>token</t>
   </si>
@@ -33,304 +33,604 @@
     <t>id</t>
   </si>
   <si>
+    <t>feel</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>rather</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>chart</t>
+  </si>
+  <si>
+    <t>polici</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>industri</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
     <t>particular</t>
   </si>
   <si>
+    <t>sever</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>employ</t>
+  </si>
+  <si>
+    <t>rate</t>
+  </si>
+  <si>
+    <t>hear</t>
+  </si>
+  <si>
+    <t>governor</t>
+  </si>
+  <si>
+    <t>consum</t>
+  </si>
+  <si>
+    <t>capit</t>
+  </si>
+  <si>
+    <t>gnp</t>
+  </si>
+  <si>
+    <t>activ</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
     <t>term</t>
   </si>
   <si>
+    <t>mayb</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>higher</t>
+  </si>
+  <si>
+    <t>without</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>growth</t>
+  </si>
+  <si>
+    <t>use</t>
+  </si>
+  <si>
+    <t>someth</t>
+  </si>
+  <si>
+    <t>sort</t>
+  </si>
+  <si>
+    <t>export</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>ago</t>
+  </si>
+  <si>
+    <t>can</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>issu</t>
+  </si>
+  <si>
+    <t>look</t>
+  </si>
+  <si>
+    <t>discuss</t>
+  </si>
+  <si>
+    <t>enough</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>figur</t>
+  </si>
+  <si>
+    <t>busi</t>
+  </si>
+  <si>
+    <t>coupl</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>thing</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>half</t>
+  </si>
+  <si>
+    <t>mention</t>
+  </si>
+  <si>
+    <t>find</t>
+  </si>
+  <si>
+    <t>perhap</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>got</t>
+  </si>
+  <si>
+    <t>strength</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>increas</t>
+  </si>
+  <si>
+    <t>signific</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>recess</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>monetari</t>
+  </si>
+  <si>
+    <t>stori</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>interest</t>
+  </si>
+  <si>
+    <t>guess</t>
+  </si>
+  <si>
+    <t>earlier</t>
+  </si>
+  <si>
+    <t>need</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>concern</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>declin</t>
+  </si>
+  <si>
+    <t>weak</t>
+  </si>
+  <si>
+    <t>real</t>
+  </si>
+  <si>
+    <t>seri</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>staff</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>risk</t>
+  </si>
+  <si>
+    <t>agre</t>
+  </si>
+  <si>
+    <t>much</t>
+  </si>
+  <si>
+    <t>effect</t>
+  </si>
+  <si>
+    <t>pick</t>
+  </si>
+  <si>
+    <t>accumul</t>
+  </si>
+  <si>
+    <t>peopl</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>larg</t>
+  </si>
+  <si>
+    <t>whole</t>
+  </si>
+  <si>
+    <t>indic</t>
+  </si>
+  <si>
+    <t>mike</t>
+  </si>
+  <si>
+    <t>develop</t>
+  </si>
+  <si>
+    <t>big</t>
+  </si>
+  <si>
+    <t>somewhat</t>
+  </si>
+  <si>
+    <t>equip</t>
+  </si>
+  <si>
+    <t>quit</t>
+  </si>
+  <si>
+    <t>tell</t>
+  </si>
+  <si>
+    <t>longer</t>
+  </si>
+  <si>
+    <t>inventori</t>
+  </si>
+  <si>
+    <t>realli</t>
+  </si>
+  <si>
+    <t>give</t>
+  </si>
+  <si>
+    <t>weaker</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>dollar</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>lot</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
     <t>seem</t>
   </si>
   <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>assumpt</t>
+  </si>
+  <si>
     <t>inflat</t>
   </si>
   <si>
+    <t>pretti</t>
+  </si>
+  <si>
+    <t>domest</t>
+  </si>
+  <si>
+    <t>lead</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>certain</t>
+  </si>
+  <si>
     <t>mr</t>
   </si>
   <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>sector</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>will</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
+  <si>
+    <t>presid</t>
+  </si>
+  <si>
+    <t>worri</t>
+  </si>
+  <si>
+    <t>extent</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>happen</t>
+  </si>
+  <si>
+    <t>hand</t>
+  </si>
+  <si>
+    <t>talk</t>
+  </si>
+  <si>
+    <t>market</t>
+  </si>
+  <si>
+    <t>steel</t>
+  </si>
+  <si>
+    <t>adjust</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>cannot</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>tri</t>
+  </si>
+  <si>
+    <t>show</t>
+  </si>
+  <si>
+    <t>invest</t>
+  </si>
+  <si>
     <t>economi</t>
   </si>
   <si>
+    <t>nation</t>
+  </si>
+  <si>
+    <t>slow</t>
+  </si>
+  <si>
+    <t>capac</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>want</t>
+  </si>
+  <si>
+    <t>slower</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>chairman</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>basic</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>probabl</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>improv</t>
+  </si>
+  <si>
+    <t>retail</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>financi</t>
+  </si>
+  <si>
+    <t>manufactur</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>run</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>given</t>
+  </si>
+  <si>
+    <t>exampl</t>
+  </si>
+  <si>
+    <t>littl</t>
+  </si>
+  <si>
+    <t>far</t>
+  </si>
+  <si>
+    <t>around</t>
+  </si>
+  <si>
+    <t>come</t>
+  </si>
+  <si>
+    <t>cours</t>
+  </si>
+  <si>
+    <t>spend</t>
+  </si>
+  <si>
+    <t>quarter</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
+    <t>tend</t>
+  </si>
+  <si>
+    <t>might</t>
+  </si>
+  <si>
     <t>price</t>
   </si>
   <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>weak</t>
-  </si>
-  <si>
-    <t>know</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>probabl</t>
-  </si>
-  <si>
-    <t>question</t>
+    <t>think</t>
+  </si>
+  <si>
+    <t>greater</t>
+  </si>
+  <si>
+    <t>chang</t>
+  </si>
+  <si>
+    <t>forecast</t>
+  </si>
+  <si>
+    <t>let</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>fact</t>
+  </si>
+  <si>
+    <t>sens</t>
+  </si>
+  <si>
+    <t>regard</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>oper</t>
+  </si>
+  <si>
+    <t>cycl</t>
+  </si>
+  <si>
+    <t>fourth</t>
+  </si>
+  <si>
+    <t>expect</t>
   </si>
   <si>
     <t>part</t>
   </si>
   <si>
-    <t>polici</t>
-  </si>
-  <si>
-    <t>thing</t>
-  </si>
-  <si>
-    <t>signific</t>
-  </si>
-  <si>
-    <t>next</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>sector</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
-    <t>market</t>
-  </si>
-  <si>
-    <t>move</t>
-  </si>
-  <si>
-    <t>thank</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>forecast</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
-    <t>greenbook</t>
-  </si>
-  <si>
-    <t>much</t>
-  </si>
-  <si>
-    <t>effect</t>
-  </si>
-  <si>
-    <t>recent</t>
-  </si>
-  <si>
-    <t>point</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>spend</t>
-  </si>
-  <si>
-    <t>expect</t>
-  </si>
-  <si>
-    <t>rate</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>rise</t>
-  </si>
-  <si>
-    <t>sale</t>
-  </si>
-  <si>
-    <t>littl</t>
-  </si>
-  <si>
-    <t>come</t>
-  </si>
-  <si>
-    <t>chang</t>
-  </si>
-  <si>
     <t>differ</t>
-  </si>
-  <si>
-    <t>can</t>
-  </si>
-  <si>
-    <t>larg</t>
-  </si>
-  <si>
-    <t>strong</t>
-  </si>
-  <si>
-    <t>dollar</t>
-  </si>
-  <si>
-    <t>chairman</t>
-  </si>
-  <si>
-    <t>percent</t>
-  </si>
-  <si>
-    <t>risk</t>
-  </si>
-  <si>
-    <t>indic</t>
-  </si>
-  <si>
-    <t>side</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>outlook</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>employ</t>
-  </si>
-  <si>
-    <t>activ</t>
-  </si>
-  <si>
-    <t>remain</t>
-  </si>
-  <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>demand</t>
-  </si>
-  <si>
-    <t>quarter</t>
-  </si>
-  <si>
-    <t>might</t>
-  </si>
-  <si>
-    <t>import</t>
-  </si>
-  <si>
-    <t>higher</t>
-  </si>
-  <si>
-    <t>peopl</t>
-  </si>
-  <si>
-    <t>lot</t>
-  </si>
-  <si>
-    <t>firm</t>
-  </si>
-  <si>
-    <t>show</t>
-  </si>
-  <si>
-    <t>report</t>
-  </si>
-  <si>
-    <t>meet</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>certain</t>
-  </si>
-  <si>
-    <t>will</t>
-  </si>
-  <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>nation</t>
-  </si>
-  <si>
-    <t>view</t>
-  </si>
-  <si>
-    <t>interest</t>
-  </si>
-  <si>
-    <t>real</t>
-  </si>
-  <si>
-    <t>district</t>
-  </si>
-  <si>
-    <t>manufactur</t>
-  </si>
-  <si>
-    <t>relat</t>
-  </si>
-  <si>
-    <t>project</t>
-  </si>
-  <si>
-    <t>last</t>
-  </si>
-  <si>
-    <t>look</t>
-  </si>
-  <si>
-    <t>busi</t>
-  </si>
-  <si>
-    <t>quit</t>
-  </si>
-  <si>
-    <t>continu</t>
-  </si>
-  <si>
-    <t>suggest</t>
-  </si>
-  <si>
-    <t>slow</t>
-  </si>
-  <si>
-    <t>improv</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>industri</t>
-  </si>
-  <si>
-    <t>increas</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>reason</t>
-  </si>
-  <si>
-    <t>concern</t>
-  </si>
-  <si>
-    <t>inventori</t>
-  </si>
-  <si>
-    <t>growth</t>
-  </si>
-  <si>
-    <t>think</t>
-  </si>
-  <si>
-    <t>declin</t>
   </si>
 </sst>
 </file>
@@ -682,7 +982,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1496,6 +1796,806 @@
         <v>100</v>
       </c>
     </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>152</v>
+      </c>
+      <c r="B152">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" t="s">
+        <v>159</v>
+      </c>
+      <c r="B159">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" t="s">
+        <v>160</v>
+      </c>
+      <c r="B160">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" t="s">
+        <v>162</v>
+      </c>
+      <c r="B162">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" t="s">
+        <v>163</v>
+      </c>
+      <c r="B163">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" t="s">
+        <v>166</v>
+      </c>
+      <c r="B166">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>169</v>
+      </c>
+      <c r="B169">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>170</v>
+      </c>
+      <c r="B170">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>172</v>
+      </c>
+      <c r="B172">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>173</v>
+      </c>
+      <c r="B173">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>174</v>
+      </c>
+      <c r="B174">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>175</v>
+      </c>
+      <c r="B175">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>176</v>
+      </c>
+      <c r="B176">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>177</v>
+      </c>
+      <c r="B177">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>178</v>
+      </c>
+      <c r="B178">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>179</v>
+      </c>
+      <c r="B179">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>180</v>
+      </c>
+      <c r="B180">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>181</v>
+      </c>
+      <c r="B181">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>182</v>
+      </c>
+      <c r="B182">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>183</v>
+      </c>
+      <c r="B183">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>184</v>
+      </c>
+      <c r="B184">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>185</v>
+      </c>
+      <c r="B185">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>186</v>
+      </c>
+      <c r="B186">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>187</v>
+      </c>
+      <c r="B187">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>188</v>
+      </c>
+      <c r="B188">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>189</v>
+      </c>
+      <c r="B189">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>190</v>
+      </c>
+      <c r="B190">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>191</v>
+      </c>
+      <c r="B191">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>192</v>
+      </c>
+      <c r="B192">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>193</v>
+      </c>
+      <c r="B193">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>194</v>
+      </c>
+      <c r="B194">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>195</v>
+      </c>
+      <c r="B195">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>196</v>
+      </c>
+      <c r="B196">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>197</v>
+      </c>
+      <c r="B197">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
+        <v>198</v>
+      </c>
+      <c r="B198">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>199</v>
+      </c>
+      <c r="B199">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>200</v>
+      </c>
+      <c r="B200">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>201</v>
+      </c>
+      <c r="B201">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>